<commit_message>
Updated ITA model - 2025-08-16 11:57
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FC395E2-BF1E-4472-9490-7F579D28DAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FDF15E7-6FEE-4882-B48A-96B6FA9502E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="misc" sheetId="7" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="EV Battery" sheetId="10" r:id="rId4"/>
     <sheet name="solar" sheetId="11" r:id="rId5"/>
     <sheet name="wind" sheetId="12" r:id="rId6"/>
+    <sheet name="conventional" sheetId="13" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1778" uniqueCount="412">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -658,18 +659,18 @@
     <t>solar resource -- CF class spv-ITA_13 -- cost class 3</t>
   </si>
   <si>
+    <t>e_spv-ITA_13_c2</t>
+  </si>
+  <si>
+    <t>solar resource -- CF class spv-ITA_13 -- cost class 2</t>
+  </si>
+  <si>
     <t>e_spv-ITA_13_c4</t>
   </si>
   <si>
     <t>solar resource -- CF class spv-ITA_13 -- cost class 4</t>
   </si>
   <si>
-    <t>e_spv-ITA_13_c2</t>
-  </si>
-  <si>
-    <t>solar resource -- CF class spv-ITA_13 -- cost class 2</t>
-  </si>
-  <si>
     <t>comm-out</t>
   </si>
   <si>
@@ -748,6 +749,12 @@
     <t>wind resource -- CF class won-ITA_29 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-ITA_29_c4</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_29 -- cost class 4</t>
+  </si>
+  <si>
     <t>e_won-ITA_29_c5</t>
   </si>
   <si>
@@ -760,12 +767,6 @@
     <t>wind resource -- CF class won-ITA_29 -- cost class 3</t>
   </si>
   <si>
-    <t>e_won-ITA_29_c4</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_29 -- cost class 4</t>
-  </si>
-  <si>
     <t>e_won-ITA_28_c1</t>
   </si>
   <si>
@@ -808,16 +809,22 @@
     <t>wind resource -- CF class won-ITA_26 -- cost class 2</t>
   </si>
   <si>
+    <t>e_won-ITA_25_c2</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_25 -- cost class 2</t>
+  </si>
+  <si>
     <t>e_won-ITA_25_c1</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_25 -- cost class 1</t>
   </si>
   <si>
-    <t>e_won-ITA_25_c2</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_25 -- cost class 2</t>
+    <t>e_won-ITA_25_c4</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_25 -- cost class 4</t>
   </si>
   <si>
     <t>e_won-ITA_25_c3</t>
@@ -826,12 +833,6 @@
     <t>wind resource -- CF class won-ITA_25 -- cost class 3</t>
   </si>
   <si>
-    <t>e_won-ITA_25_c4</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_25 -- cost class 4</t>
-  </si>
-  <si>
     <t>e_won-ITA_24_c2</t>
   </si>
   <si>
@@ -1222,6 +1223,12 @@
     <t>wind resource -- CF class won-ITA_12 -- cost class 2</t>
   </si>
   <si>
+    <t>e_won-ITA_11_c2</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_11 -- cost class 2</t>
+  </si>
+  <si>
     <t>e_won-ITA_11_c4</t>
   </si>
   <si>
@@ -1234,12 +1241,6 @@
     <t>wind resource -- CF class won-ITA_11 -- cost class 5</t>
   </si>
   <si>
-    <t>e_won-ITA_11_c2</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_11 -- cost class 2</t>
-  </si>
-  <si>
     <t>e_won-ITA_11_c1</t>
   </si>
   <si>
@@ -1252,19 +1253,94 @@
     <t>wind resource -- CF class won-ITA_11 -- cost class 3</t>
   </si>
   <si>
+    <t>e_won-ITA_10_c1</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_10 -- cost class 1</t>
+  </si>
+  <si>
     <t>e_won-ITA_10_c2</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_10 -- cost class 2</t>
   </si>
   <si>
-    <t>e_won-ITA_10_c1</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_10 -- cost class 1</t>
-  </si>
-  <si>
     <t>elc_won-ITA</t>
+  </si>
+  <si>
+    <t>comm-in</t>
+  </si>
+  <si>
+    <t>Bioenergy + CCUS</t>
+  </si>
+  <si>
+    <t>efficiency</t>
+  </si>
+  <si>
+    <t>ncap_af</t>
+  </si>
+  <si>
+    <t>ncap_cost</t>
+  </si>
+  <si>
+    <t>ncap_fom</t>
+  </si>
+  <si>
+    <t>ncap_iled</t>
+  </si>
+  <si>
+    <t>Bioenergy - Large scale unit</t>
+  </si>
+  <si>
+    <t>CCGT</t>
+  </si>
+  <si>
+    <t>CCGT + CCS</t>
+  </si>
+  <si>
+    <t>Coal + CCS</t>
+  </si>
+  <si>
+    <t>Gas turbine</t>
+  </si>
+  <si>
+    <t>Hydropower - large-scale unit</t>
+  </si>
+  <si>
+    <t>IGCC</t>
+  </si>
+  <si>
+    <t>IGCC + CCS</t>
+  </si>
+  <si>
+    <t>Nuclear large</t>
+  </si>
+  <si>
+    <t>Oxyfuel + CCS</t>
+  </si>
+  <si>
+    <t>Solar photovoltaics - Large scale unit</t>
+  </si>
+  <si>
+    <t>Steam Coal - SUBCRITICAL</t>
+  </si>
+  <si>
+    <t>Steam Coal - SUPERCRITICAL</t>
+  </si>
+  <si>
+    <t>Steam Coal - ULTRASUPERCRITICAL</t>
+  </si>
+  <si>
+    <t>Wind offshore</t>
+  </si>
+  <si>
+    <t>Wind onshore</t>
+  </si>
+  <si>
+    <t>daynite</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -1640,7 +1716,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{947D673D-527F-ECF8-871B-AB13FFADE98E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30CB1E2D-16D1-7F5C-3E8D-2FEC70133023}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1695,7 +1771,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92309C50-36CB-8BDF-D63F-7FB9C9B46F59}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AA2F103-5300-E3E9-4AAD-9D6B32B94D3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1750,7 +1826,62 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A0BB5EB-2EEB-83C7-8CF5-418DE115C921}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{749D1D58-13AF-C87E-7884-9F8B02BE9EB1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5245100" y="12700"/>
+          <a:ext cx="990600" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1D9B3EE-63E2-2708-AA79-3947C8DA3A5D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4253,7 +4384,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF7AD31-B357-46C8-9C76-4151F605503E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEBD5B3D-799E-4002-8504-3F575121DCEA}">
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5481,7 +5612,7 @@
         <v>64.217124244118722</v>
       </c>
       <c r="P31" s="33">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="2:16">
@@ -5522,7 +5653,7 @@
         <v>64.217124244118722</v>
       </c>
       <c r="P32" s="32">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -5535,10 +5666,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545F1935-CE42-48CD-BA45-6BE709CADD20}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DBE7B01-01BC-424A-8D05-7B9FCD15ABB5}">
   <dimension ref="A1:P99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -6064,7 +6197,7 @@
         <v>61.739678606582956</v>
       </c>
       <c r="P14" s="32">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -6105,7 +6238,7 @@
         <v>61.739678606582956</v>
       </c>
       <c r="P15" s="33">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -6146,7 +6279,7 @@
         <v>61.739678606582956</v>
       </c>
       <c r="P16" s="32">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:16">
@@ -6474,7 +6607,7 @@
         <v>39.368264706413946</v>
       </c>
       <c r="P24" s="32">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="2:16">
@@ -6515,7 +6648,7 @@
         <v>39.368264706413946</v>
       </c>
       <c r="P25" s="33">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:16">
@@ -6547,16 +6680,16 @@
         <v>386</v>
       </c>
       <c r="M26" s="32">
-        <v>3.2032500000000002</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="N26" s="34">
         <v>0.245</v>
       </c>
       <c r="O26" s="35">
-        <v>42.969340484621256</v>
+        <v>107.03467623779731</v>
       </c>
       <c r="P26" s="32">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="2:16">
@@ -6588,16 +6721,16 @@
         <v>386</v>
       </c>
       <c r="M27" s="33">
-        <v>4.4999999999999997E-3</v>
+        <v>3.2032500000000002</v>
       </c>
       <c r="N27" s="36">
         <v>0.245</v>
       </c>
       <c r="O27" s="37">
-        <v>107.03467623779731</v>
+        <v>42.969340484621256</v>
       </c>
       <c r="P27" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="2:16">
@@ -9294,16 +9427,16 @@
         <v>386</v>
       </c>
       <c r="M93" s="33">
-        <v>0.43575000000000003</v>
+        <v>0.03</v>
       </c>
       <c r="N93" s="36">
         <v>0.113</v>
       </c>
       <c r="O93" s="37">
-        <v>120.30091898433189</v>
+        <v>94.983314628615091</v>
       </c>
       <c r="P93" s="33">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="2:16">
@@ -9344,7 +9477,7 @@
         <v>120.30091898433189</v>
       </c>
       <c r="P94" s="32">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="2:16">
@@ -9376,16 +9509,16 @@
         <v>386</v>
       </c>
       <c r="M95" s="33">
-        <v>0.03</v>
+        <v>0.43575000000000003</v>
       </c>
       <c r="N95" s="36">
         <v>0.113</v>
       </c>
       <c r="O95" s="37">
-        <v>94.983314628615091</v>
+        <v>120.30091898433189</v>
       </c>
       <c r="P95" s="33">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="2:16">
@@ -9508,7 +9641,7 @@
         <v>74.16840218346799</v>
       </c>
       <c r="P98" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="2:16">
@@ -9549,7 +9682,1871 @@
         <v>74.16840218346799</v>
       </c>
       <c r="P99" s="33">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A6DFD6-0928-458F-89A1-5F6D45A6FEA1}">
+  <dimension ref="A1:Q66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="27.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="10.59765625" customWidth="1"/>
+    <col min="11" max="11" width="10.59765625" customWidth="1"/>
+    <col min="12" max="12" width="27.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.59765625" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.46484375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="22.05" customHeight="1">
+      <c r="A1" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+    </row>
+    <row r="2" spans="1:17" ht="14.65" thickBot="1">
+      <c r="B2" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" thickBot="1">
+      <c r="B3" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>387</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="E3" s="29">
+        <v>2023</v>
+      </c>
+      <c r="F3" s="29">
+        <v>2030</v>
+      </c>
+      <c r="G3" s="29">
+        <v>2050</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="L3" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="M3" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="N3" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="O3" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="P3" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q3" s="29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="B4" s="30" t="s">
+        <v>388</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="35">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="F4" s="35">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="G4" s="35">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>389</v>
+      </c>
+      <c r="K4" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="L4" s="30" t="s">
+        <v>388</v>
+      </c>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="30" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q4" s="30" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="B5" s="31" t="s">
+        <v>388</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="37">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="F5" s="37">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="G5" s="37">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>390</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="L5" s="31" t="s">
+        <v>394</v>
+      </c>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" s="31" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q5" s="31" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="B6" s="30" t="s">
+        <v>388</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="35">
+        <v>5750</v>
+      </c>
+      <c r="F6" s="35">
+        <v>5700</v>
+      </c>
+      <c r="G6" s="35">
+        <v>5100</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>391</v>
+      </c>
+      <c r="K6" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="L6" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="P6" s="30" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q6" s="30" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="B7" s="31" t="s">
+        <v>388</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="37">
+        <v>200</v>
+      </c>
+      <c r="F7" s="37">
+        <v>200</v>
+      </c>
+      <c r="G7" s="37">
+        <v>175</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>392</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="L7" s="31" t="s">
+        <v>396</v>
+      </c>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" s="31" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q7" s="31" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="B8" s="30" t="s">
+        <v>388</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="35">
+        <v>3</v>
+      </c>
+      <c r="F8" s="35">
+        <v>3</v>
+      </c>
+      <c r="G8" s="35">
+        <v>3</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>393</v>
+      </c>
+      <c r="K8" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="L8" s="30" t="s">
+        <v>397</v>
+      </c>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="O8" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="P8" s="30" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q8" s="30" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="B9" s="31" t="s">
+        <v>394</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="37">
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="F9" s="37">
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="G9" s="37">
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>389</v>
+      </c>
+      <c r="K9" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="L9" s="31" t="s">
+        <v>398</v>
+      </c>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O9" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="P9" s="31" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q9" s="31" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="B10" s="30" t="s">
+        <v>394</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="35">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="F10" s="35">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="G10" s="35">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>390</v>
+      </c>
+      <c r="K10" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="L10" s="30" t="s">
+        <v>399</v>
+      </c>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="O10" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10" s="30" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q10" s="30" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="B11" s="31" t="s">
+        <v>394</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="37">
+        <v>2400</v>
+      </c>
+      <c r="F11" s="37">
+        <v>2350</v>
+      </c>
+      <c r="G11" s="37">
+        <v>2300</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>391</v>
+      </c>
+      <c r="K11" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="L11" s="31" t="s">
+        <v>400</v>
+      </c>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" s="31" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q11" s="31" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="B12" s="30" t="s">
+        <v>394</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="35">
+        <v>85</v>
+      </c>
+      <c r="F12" s="35">
+        <v>85</v>
+      </c>
+      <c r="G12" s="35">
+        <v>80</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>392</v>
+      </c>
+      <c r="K12" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="L12" s="30" t="s">
+        <v>401</v>
+      </c>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="O12" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" s="30" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q12" s="30" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="B13" s="31" t="s">
+        <v>394</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="37">
+        <v>3</v>
+      </c>
+      <c r="F13" s="37">
+        <v>3</v>
+      </c>
+      <c r="G13" s="37">
+        <v>3</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>393</v>
+      </c>
+      <c r="K13" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="L13" s="31" t="s">
+        <v>402</v>
+      </c>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O13" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="P13" s="31" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q13" s="31" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="B14" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="35">
+        <v>0.59</v>
+      </c>
+      <c r="F14" s="35">
+        <v>0.6</v>
+      </c>
+      <c r="G14" s="35">
+        <v>0.61</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>389</v>
+      </c>
+      <c r="K14" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="L14" s="30" t="s">
+        <v>403</v>
+      </c>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="O14" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="P14" s="30" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q14" s="30" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="B15" s="31" t="s">
+        <v>395</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="37">
+        <v>1000</v>
+      </c>
+      <c r="F15" s="37">
+        <v>1000</v>
+      </c>
+      <c r="G15" s="37">
+        <v>1000</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>391</v>
+      </c>
+      <c r="K15" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="L15" s="31" t="s">
+        <v>404</v>
+      </c>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O15" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="P15" s="31" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q15" s="31" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="B16" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="35">
+        <v>25</v>
+      </c>
+      <c r="F16" s="35">
+        <v>25</v>
+      </c>
+      <c r="G16" s="35">
+        <v>25</v>
+      </c>
+      <c r="H16" s="30" t="s">
+        <v>392</v>
+      </c>
+      <c r="K16" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="L16" s="30" t="s">
+        <v>405</v>
+      </c>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="O16" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="P16" s="30" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q16" s="30" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17">
+      <c r="B17" s="31" t="s">
+        <v>396</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="37">
+        <v>0.51</v>
+      </c>
+      <c r="F17" s="37">
+        <v>0.52</v>
+      </c>
+      <c r="G17" s="37">
+        <v>0.54</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>389</v>
+      </c>
+      <c r="K17" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="L17" s="31" t="s">
+        <v>406</v>
+      </c>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O17" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="P17" s="31" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q17" s="31" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17">
+      <c r="B18" s="30" t="s">
+        <v>396</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="35">
+        <v>3100</v>
+      </c>
+      <c r="F18" s="35">
+        <v>3100</v>
+      </c>
+      <c r="G18" s="35">
+        <v>2400</v>
+      </c>
+      <c r="H18" s="30" t="s">
+        <v>391</v>
+      </c>
+      <c r="K18" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="L18" s="30" t="s">
+        <v>407</v>
+      </c>
+      <c r="M18" s="30"/>
+      <c r="N18" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="O18" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="P18" s="30" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q18" s="30" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17">
+      <c r="B19" s="31" t="s">
+        <v>396</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="37">
+        <v>75</v>
+      </c>
+      <c r="F19" s="37">
+        <v>75</v>
+      </c>
+      <c r="G19" s="37">
+        <v>60</v>
+      </c>
+      <c r="H19" s="31" t="s">
+        <v>392</v>
+      </c>
+      <c r="K19" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="L19" s="31" t="s">
+        <v>408</v>
+      </c>
+      <c r="M19" s="31"/>
+      <c r="N19" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O19" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="P19" s="31" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q19" s="31" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17">
+      <c r="B20" s="30" t="s">
+        <v>397</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="35">
+        <v>0.37</v>
+      </c>
+      <c r="F20" s="35">
+        <v>0.38</v>
+      </c>
+      <c r="G20" s="35">
+        <v>0.39</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>389</v>
+      </c>
+      <c r="K20" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="L20" s="30" t="s">
+        <v>409</v>
+      </c>
+      <c r="M20" s="30"/>
+      <c r="N20" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="O20" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="P20" s="30" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q20" s="30" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17">
+      <c r="B21" s="31" t="s">
+        <v>397</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="37">
+        <v>5500</v>
+      </c>
+      <c r="F21" s="37">
+        <v>5500</v>
+      </c>
+      <c r="G21" s="37">
+        <v>4350</v>
+      </c>
+      <c r="H21" s="31" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17">
+      <c r="B22" s="30" t="s">
+        <v>397</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="35">
+        <v>165</v>
+      </c>
+      <c r="F22" s="35">
+        <v>165</v>
+      </c>
+      <c r="G22" s="35">
+        <v>130</v>
+      </c>
+      <c r="H22" s="30" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17">
+      <c r="B23" s="31" t="s">
+        <v>398</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="37">
+        <v>0.4</v>
+      </c>
+      <c r="F23" s="37">
+        <v>0.41000000000000003</v>
+      </c>
+      <c r="G23" s="37">
+        <v>0.42</v>
+      </c>
+      <c r="H23" s="31" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17">
+      <c r="B24" s="30" t="s">
+        <v>398</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="35">
+        <v>500</v>
+      </c>
+      <c r="F24" s="35">
+        <v>500</v>
+      </c>
+      <c r="G24" s="35">
+        <v>500</v>
+      </c>
+      <c r="H24" s="30" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17">
+      <c r="B25" s="31" t="s">
+        <v>398</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="37">
+        <v>20</v>
+      </c>
+      <c r="F25" s="37">
+        <v>20</v>
+      </c>
+      <c r="G25" s="37">
+        <v>20</v>
+      </c>
+      <c r="H25" s="31" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17">
+      <c r="B26" s="30" t="s">
+        <v>399</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="35">
         <v>1</v>
+      </c>
+      <c r="F26" s="35">
+        <v>1</v>
+      </c>
+      <c r="G26" s="35">
+        <v>1</v>
+      </c>
+      <c r="H26" s="30" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17">
+      <c r="B27" s="31" t="s">
+        <v>399</v>
+      </c>
+      <c r="C27" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="37">
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="F27" s="37">
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="G27" s="37">
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="H27" s="31" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17">
+      <c r="B28" s="30" t="s">
+        <v>399</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="35">
+        <v>2650</v>
+      </c>
+      <c r="F28" s="35">
+        <v>2650</v>
+      </c>
+      <c r="G28" s="35">
+        <v>2650</v>
+      </c>
+      <c r="H28" s="30" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17">
+      <c r="B29" s="31" t="s">
+        <v>399</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="37">
+        <v>65</v>
+      </c>
+      <c r="F29" s="37">
+        <v>65</v>
+      </c>
+      <c r="G29" s="37">
+        <v>65</v>
+      </c>
+      <c r="H29" s="31" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17">
+      <c r="B30" s="30" t="s">
+        <v>399</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="35">
+        <v>4</v>
+      </c>
+      <c r="F30" s="35">
+        <v>4</v>
+      </c>
+      <c r="G30" s="35">
+        <v>4</v>
+      </c>
+      <c r="H30" s="30" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17">
+      <c r="B31" s="31" t="s">
+        <v>400</v>
+      </c>
+      <c r="C31" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="37">
+        <v>0.45</v>
+      </c>
+      <c r="F31" s="37">
+        <v>0.47000000000000003</v>
+      </c>
+      <c r="G31" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="H31" s="31" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17">
+      <c r="B32" s="30" t="s">
+        <v>400</v>
+      </c>
+      <c r="C32" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="35">
+        <v>2500</v>
+      </c>
+      <c r="F32" s="35">
+        <v>2350</v>
+      </c>
+      <c r="G32" s="35">
+        <v>2300</v>
+      </c>
+      <c r="H32" s="30" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="B33" s="31" t="s">
+        <v>400</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="37">
+        <v>95</v>
+      </c>
+      <c r="F33" s="37">
+        <v>85</v>
+      </c>
+      <c r="G33" s="37">
+        <v>80</v>
+      </c>
+      <c r="H33" s="31" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" s="30" t="s">
+        <v>401</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="35">
+        <v>0.36</v>
+      </c>
+      <c r="F34" s="35">
+        <v>0.38</v>
+      </c>
+      <c r="G34" s="35">
+        <v>0.43</v>
+      </c>
+      <c r="H34" s="30" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="31" t="s">
+        <v>401</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="37">
+        <v>5850</v>
+      </c>
+      <c r="F35" s="37">
+        <v>5700</v>
+      </c>
+      <c r="G35" s="37">
+        <v>5100</v>
+      </c>
+      <c r="H35" s="31" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="30" t="s">
+        <v>401</v>
+      </c>
+      <c r="C36" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" s="35">
+        <v>205</v>
+      </c>
+      <c r="F36" s="35">
+        <v>200</v>
+      </c>
+      <c r="G36" s="35">
+        <v>180</v>
+      </c>
+      <c r="H36" s="30" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="B37" s="31" t="s">
+        <v>402</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="37">
+        <v>0.33</v>
+      </c>
+      <c r="F37" s="37">
+        <v>0.33</v>
+      </c>
+      <c r="G37" s="37">
+        <v>0.33</v>
+      </c>
+      <c r="H37" s="31" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8">
+      <c r="B38" s="30" t="s">
+        <v>402</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" s="35">
+        <v>6600</v>
+      </c>
+      <c r="F38" s="35">
+        <v>5100</v>
+      </c>
+      <c r="G38" s="35">
+        <v>4500</v>
+      </c>
+      <c r="H38" s="30" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="31" t="s">
+        <v>402</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="37">
+        <v>165</v>
+      </c>
+      <c r="F39" s="37">
+        <v>165</v>
+      </c>
+      <c r="G39" s="37">
+        <v>160</v>
+      </c>
+      <c r="H39" s="31" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="30" t="s">
+        <v>403</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="35">
+        <v>0.37</v>
+      </c>
+      <c r="F40" s="35">
+        <v>0.38</v>
+      </c>
+      <c r="G40" s="35">
+        <v>0.39</v>
+      </c>
+      <c r="H40" s="30" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" s="31" t="s">
+        <v>403</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" s="37">
+        <v>5700</v>
+      </c>
+      <c r="F41" s="37">
+        <v>5700</v>
+      </c>
+      <c r="G41" s="37">
+        <v>5100</v>
+      </c>
+      <c r="H41" s="31" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="B42" s="30" t="s">
+        <v>403</v>
+      </c>
+      <c r="C42" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="35">
+        <v>170</v>
+      </c>
+      <c r="F42" s="35">
+        <v>170</v>
+      </c>
+      <c r="G42" s="35">
+        <v>155</v>
+      </c>
+      <c r="H42" s="30" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="31" t="s">
+        <v>404</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E43" s="37">
+        <v>1</v>
+      </c>
+      <c r="F43" s="37">
+        <v>1</v>
+      </c>
+      <c r="G43" s="37">
+        <v>1</v>
+      </c>
+      <c r="H43" s="31" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8">
+      <c r="B44" s="30" t="s">
+        <v>404</v>
+      </c>
+      <c r="C44" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" s="35">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F44" s="35">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G44" s="35">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H44" s="30" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8">
+      <c r="B45" s="31" t="s">
+        <v>404</v>
+      </c>
+      <c r="C45" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="37">
+        <v>750</v>
+      </c>
+      <c r="F45" s="37">
+        <v>480</v>
+      </c>
+      <c r="G45" s="37">
+        <v>340</v>
+      </c>
+      <c r="H45" s="31" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" s="30" t="s">
+        <v>404</v>
+      </c>
+      <c r="C46" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E46" s="35">
+        <v>12</v>
+      </c>
+      <c r="F46" s="35">
+        <v>10</v>
+      </c>
+      <c r="G46" s="35">
+        <v>10</v>
+      </c>
+      <c r="H46" s="30" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="B47" s="31" t="s">
+        <v>404</v>
+      </c>
+      <c r="C47" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D47" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47" s="37">
+        <v>1.5</v>
+      </c>
+      <c r="F47" s="37">
+        <v>1.5</v>
+      </c>
+      <c r="G47" s="37">
+        <v>1.5</v>
+      </c>
+      <c r="H47" s="31" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8">
+      <c r="B48" s="30" t="s">
+        <v>405</v>
+      </c>
+      <c r="C48" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E48" s="35">
+        <v>0.39</v>
+      </c>
+      <c r="F48" s="35">
+        <v>0.39</v>
+      </c>
+      <c r="G48" s="35">
+        <v>0.39</v>
+      </c>
+      <c r="H48" s="30" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8">
+      <c r="B49" s="31" t="s">
+        <v>405</v>
+      </c>
+      <c r="C49" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D49" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E49" s="37">
+        <v>1700</v>
+      </c>
+      <c r="F49" s="37">
+        <v>1700</v>
+      </c>
+      <c r="G49" s="37">
+        <v>1700</v>
+      </c>
+      <c r="H49" s="31" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8">
+      <c r="B50" s="30" t="s">
+        <v>405</v>
+      </c>
+      <c r="C50" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D50" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="35">
+        <v>45</v>
+      </c>
+      <c r="F50" s="35">
+        <v>45</v>
+      </c>
+      <c r="G50" s="35">
+        <v>45</v>
+      </c>
+      <c r="H50" s="30" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8">
+      <c r="B51" s="31" t="s">
+        <v>406</v>
+      </c>
+      <c r="C51" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D51" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="37">
+        <v>0.43</v>
+      </c>
+      <c r="F51" s="37">
+        <v>0.43</v>
+      </c>
+      <c r="G51" s="37">
+        <v>0.43</v>
+      </c>
+      <c r="H51" s="31" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8">
+      <c r="B52" s="30" t="s">
+        <v>406</v>
+      </c>
+      <c r="C52" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="35">
+        <v>2000</v>
+      </c>
+      <c r="F52" s="35">
+        <v>2000</v>
+      </c>
+      <c r="G52" s="35">
+        <v>2000</v>
+      </c>
+      <c r="H52" s="30" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8">
+      <c r="B53" s="31" t="s">
+        <v>406</v>
+      </c>
+      <c r="C53" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D53" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="37">
+        <v>60</v>
+      </c>
+      <c r="F53" s="37">
+        <v>60</v>
+      </c>
+      <c r="G53" s="37">
+        <v>60</v>
+      </c>
+      <c r="H53" s="31" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8">
+      <c r="B54" s="30" t="s">
+        <v>407</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="35">
+        <v>0.46</v>
+      </c>
+      <c r="F54" s="35">
+        <v>0.46</v>
+      </c>
+      <c r="G54" s="35">
+        <v>0.48</v>
+      </c>
+      <c r="H54" s="30" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8">
+      <c r="B55" s="31" t="s">
+        <v>407</v>
+      </c>
+      <c r="C55" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D55" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E55" s="37">
+        <v>2200</v>
+      </c>
+      <c r="F55" s="37">
+        <v>2200</v>
+      </c>
+      <c r="G55" s="37">
+        <v>2200</v>
+      </c>
+      <c r="H55" s="31" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8">
+      <c r="B56" s="30" t="s">
+        <v>407</v>
+      </c>
+      <c r="C56" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D56" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56" s="35">
+        <v>65</v>
+      </c>
+      <c r="F56" s="35">
+        <v>65</v>
+      </c>
+      <c r="G56" s="35">
+        <v>65</v>
+      </c>
+      <c r="H56" s="30" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8">
+      <c r="B57" s="31" t="s">
+        <v>408</v>
+      </c>
+      <c r="C57" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D57" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" s="37">
+        <v>1</v>
+      </c>
+      <c r="F57" s="37">
+        <v>1</v>
+      </c>
+      <c r="G57" s="37">
+        <v>1</v>
+      </c>
+      <c r="H57" s="31" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8">
+      <c r="B58" s="30" t="s">
+        <v>408</v>
+      </c>
+      <c r="C58" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D58" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E58" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="F58" s="35">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G58" s="35">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H58" s="30" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8">
+      <c r="B59" s="31" t="s">
+        <v>408</v>
+      </c>
+      <c r="C59" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D59" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="37">
+        <v>3120</v>
+      </c>
+      <c r="F59" s="37">
+        <v>2280</v>
+      </c>
+      <c r="G59" s="37">
+        <v>1660</v>
+      </c>
+      <c r="H59" s="31" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8">
+      <c r="B60" s="30" t="s">
+        <v>408</v>
+      </c>
+      <c r="C60" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D60" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" s="35">
+        <v>60</v>
+      </c>
+      <c r="F60" s="35">
+        <v>50</v>
+      </c>
+      <c r="G60" s="35">
+        <v>40</v>
+      </c>
+      <c r="H60" s="30" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8">
+      <c r="B61" s="31" t="s">
+        <v>408</v>
+      </c>
+      <c r="C61" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D61" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E61" s="37">
+        <v>3</v>
+      </c>
+      <c r="F61" s="37">
+        <v>3</v>
+      </c>
+      <c r="G61" s="37">
+        <v>3</v>
+      </c>
+      <c r="H61" s="31" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8">
+      <c r="B62" s="30" t="s">
+        <v>409</v>
+      </c>
+      <c r="C62" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D62" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E62" s="35">
+        <v>1</v>
+      </c>
+      <c r="F62" s="35">
+        <v>1</v>
+      </c>
+      <c r="G62" s="35">
+        <v>1</v>
+      </c>
+      <c r="H62" s="30" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8">
+      <c r="B63" s="31" t="s">
+        <v>409</v>
+      </c>
+      <c r="C63" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D63" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E63" s="37">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F63" s="37">
+        <v>0.3</v>
+      </c>
+      <c r="G63" s="37">
+        <v>0.3</v>
+      </c>
+      <c r="H63" s="31" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8">
+      <c r="B64" s="30" t="s">
+        <v>409</v>
+      </c>
+      <c r="C64" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D64" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E64" s="35">
+        <v>1630</v>
+      </c>
+      <c r="F64" s="35">
+        <v>1550</v>
+      </c>
+      <c r="G64" s="35">
+        <v>1490</v>
+      </c>
+      <c r="H64" s="30" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8">
+      <c r="B65" s="31" t="s">
+        <v>409</v>
+      </c>
+      <c r="C65" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D65" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E65" s="37">
+        <v>42</v>
+      </c>
+      <c r="F65" s="37">
+        <v>40</v>
+      </c>
+      <c r="G65" s="37">
+        <v>38</v>
+      </c>
+      <c r="H65" s="31" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8">
+      <c r="B66" s="30" t="s">
+        <v>409</v>
+      </c>
+      <c r="C66" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D66" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E66" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="F66" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="G66" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="H66" s="30" t="s">
+        <v>393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-17 21:20
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A369E1D-260E-4EFD-AB88-8A076F249475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1B5380E-97F3-431F-8A7D-6A807897D3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -668,18 +668,18 @@
     <t>solar resource -- CF class spv-ITA_13 -- cost class 2</t>
   </si>
   <si>
+    <t>e_spv-ITA_13_c4</t>
+  </si>
+  <si>
+    <t>solar resource -- CF class spv-ITA_13 -- cost class 4</t>
+  </si>
+  <si>
     <t>e_spv-ITA_13_c3</t>
   </si>
   <si>
     <t>solar resource -- CF class spv-ITA_13 -- cost class 3</t>
   </si>
   <si>
-    <t>e_spv-ITA_13_c4</t>
-  </si>
-  <si>
-    <t>solar resource -- CF class spv-ITA_13 -- cost class 4</t>
-  </si>
-  <si>
     <t>comm-out</t>
   </si>
   <si>
@@ -758,18 +758,18 @@
     <t>wind resource -- CF class won-ITA_29 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-ITA_29_c4</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_29 -- cost class 4</t>
+  </si>
+  <si>
     <t>e_won-ITA_29_c5</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_29 -- cost class 5</t>
   </si>
   <si>
-    <t>e_won-ITA_29_c4</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_29 -- cost class 4</t>
-  </si>
-  <si>
     <t>e_won-ITA_29_c3</t>
   </si>
   <si>
@@ -830,18 +830,18 @@
     <t>wind resource -- CF class won-ITA_25 -- cost class 2</t>
   </si>
   <si>
+    <t>e_won-ITA_25_c4</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_25 -- cost class 4</t>
+  </si>
+  <si>
     <t>e_won-ITA_25_c3</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_25 -- cost class 3</t>
   </si>
   <si>
-    <t>e_won-ITA_25_c4</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_25 -- cost class 4</t>
-  </si>
-  <si>
     <t>e_won-ITA_24_c2</t>
   </si>
   <si>
@@ -1232,6 +1232,12 @@
     <t>wind resource -- CF class won-ITA_12 -- cost class 2</t>
   </si>
   <si>
+    <t>e_won-ITA_11_c5</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_11 -- cost class 5</t>
+  </si>
+  <si>
     <t>e_won-ITA_11_c2</t>
   </si>
   <si>
@@ -1242,12 +1248,6 @@
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_11 -- cost class 4</t>
-  </si>
-  <si>
-    <t>e_won-ITA_11_c5</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_11 -- cost class 5</t>
   </si>
   <si>
     <t>e_won-ITA_11_c1</t>
@@ -1725,7 +1725,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AC712C4-CF13-DB91-0B99-E4553ED822A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA219894-5F51-84CA-8798-7101AF512E0A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1780,7 +1780,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FC3C46C-CE66-32E7-CD3D-CC12421F70AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9236A34-BB6B-C4E6-32F2-A8F78F142BFD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1835,7 +1835,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8F8CC5C-9F48-B168-11BB-11E1DC30AC41}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{842A56E0-C5AC-DA45-FF94-6AEF5BF5BE4D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1890,7 +1890,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2C5C106-A9B9-C409-0B07-3AB60D4DEFF4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{529E9AEE-EFD6-BCA1-B325-F4566AB16CD2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4417,7 +4417,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0176623-11FA-4CEE-BDDF-06E90D4CB949}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEEFD477-397C-424E-9F12-52F9E5F062DA}">
   <dimension ref="A1:P32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5645,7 +5645,7 @@
         <v>64.217124244118722</v>
       </c>
       <c r="P31" s="33">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="2:16">
@@ -5686,7 +5686,7 @@
         <v>64.217124244118722</v>
       </c>
       <c r="P32" s="32">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -5699,7 +5699,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E96730EC-B64D-41ED-BC93-CB2221D1D69A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875A24EA-1F0E-436A-975E-683F36A13B5E}">
   <dimension ref="A1:P99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6230,7 +6230,7 @@
         <v>61.739678606582956</v>
       </c>
       <c r="P14" s="32">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -6271,7 +6271,7 @@
         <v>61.739678606582956</v>
       </c>
       <c r="P15" s="33">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -6713,16 +6713,16 @@
         <v>389</v>
       </c>
       <c r="M26" s="32">
-        <v>3.2032500000000002</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="N26" s="34">
         <v>0.245</v>
       </c>
       <c r="O26" s="35">
-        <v>42.969340484621256</v>
+        <v>107.03467623779731</v>
       </c>
       <c r="P26" s="32">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="2:16">
@@ -6754,16 +6754,16 @@
         <v>389</v>
       </c>
       <c r="M27" s="33">
-        <v>4.4999999999999997E-3</v>
+        <v>3.2032500000000002</v>
       </c>
       <c r="N27" s="36">
         <v>0.245</v>
       </c>
       <c r="O27" s="37">
-        <v>107.03467623779731</v>
+        <v>42.969340484621256</v>
       </c>
       <c r="P27" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="2:16">
@@ -9460,16 +9460,16 @@
         <v>389</v>
       </c>
       <c r="M93" s="33">
-        <v>0.03</v>
+        <v>0.43575000000000003</v>
       </c>
       <c r="N93" s="36">
         <v>0.113</v>
       </c>
       <c r="O93" s="37">
-        <v>94.983314628615091</v>
+        <v>120.30091898433189</v>
       </c>
       <c r="P93" s="33">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="2:16">
@@ -9501,16 +9501,16 @@
         <v>389</v>
       </c>
       <c r="M94" s="32">
-        <v>0.43575000000000003</v>
+        <v>0.03</v>
       </c>
       <c r="N94" s="34">
         <v>0.113</v>
       </c>
       <c r="O94" s="35">
-        <v>120.30091898433189</v>
+        <v>94.983314628615091</v>
       </c>
       <c r="P94" s="32">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95" spans="2:16">
@@ -9551,7 +9551,7 @@
         <v>120.30091898433189</v>
       </c>
       <c r="P95" s="33">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="2:16">
@@ -9728,7 +9728,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C681A1-1C75-476F-A3B8-2D2680C6C1FA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC927238-405E-4772-BB16-F677370D6841}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-22 13:39
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA89C3BF-C808-4516-A51F-B181884C9D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD156EC3-D3F9-4DDA-9DE7-F3D552A4D2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -949,18 +949,18 @@
     <t>wind resource -- CF class won-ITA_25 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-ITA_25_c2</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_25 -- cost class 2</t>
+  </si>
+  <si>
     <t>e_won-ITA_25_c3</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_25 -- cost class 3</t>
   </si>
   <si>
-    <t>e_won-ITA_25_c2</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_25 -- cost class 2</t>
-  </si>
-  <si>
     <t>e_won-ITA_24_c2</t>
   </si>
   <si>
@@ -1351,16 +1351,16 @@
     <t>wind resource -- CF class won-ITA_12 -- cost class 5</t>
   </si>
   <si>
+    <t>e_won-ITA_11_c4</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_11 -- cost class 4</t>
+  </si>
+  <si>
     <t>e_won-ITA_11_c2</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_11 -- cost class 2</t>
-  </si>
-  <si>
-    <t>e_won-ITA_11_c4</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_11 -- cost class 4</t>
   </si>
   <si>
     <t>e_won-ITA_11_c1</t>
@@ -2497,7 +2497,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC459EE0-2A90-1DD8-91F2-1C330AB0FD1B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7566876-DF54-6042-4980-126A563BB9A0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2552,7 +2552,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23041752-4BD2-8116-4876-59A54C64B1A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{251245A0-B98A-3B5C-D33F-8A77E072245A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2607,7 +2607,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32FE34BE-4ED3-DCCB-64CC-0D6E93FD22F0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0612A73-9121-3AAA-23CB-68C734AFF738}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2662,7 +2662,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D9CCAEE-168B-B4D5-47F0-C19C70F6F5E4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F49161E-2F2E-E097-ED8F-E3D766AB2864}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6592,7 +6592,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{768DEBFD-919F-40EA-8E4C-49A3450457D9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11442DC-4C52-4A63-BA82-F5A1000AA215}">
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7792,7 +7792,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A91FF39-022D-4CEE-AE0A-70AC6B519573}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8896AC-B5E9-49E0-80D2-A0C817A9C078}">
   <dimension ref="A1:P94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8683,16 +8683,16 @@
         <v>417</v>
       </c>
       <c r="M23" s="159">
-        <v>4.4999999999999997E-3</v>
+        <v>3.2032500000000002</v>
       </c>
       <c r="N23" s="162">
         <v>0.245</v>
       </c>
       <c r="O23" s="163">
-        <v>107.03467623779731</v>
+        <v>42.969340484621256</v>
       </c>
       <c r="P23" s="159">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="2:16">
@@ -8724,16 +8724,16 @@
         <v>417</v>
       </c>
       <c r="M24" s="158">
-        <v>3.2032500000000002</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="N24" s="160">
         <v>0.245</v>
       </c>
       <c r="O24" s="161">
-        <v>42.969340484621256</v>
+        <v>107.03467623779731</v>
       </c>
       <c r="P24" s="158">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="2:16">
@@ -11430,16 +11430,16 @@
         <v>417</v>
       </c>
       <c r="M90" s="158">
-        <v>0.03</v>
+        <v>0.43575000000000003</v>
       </c>
       <c r="N90" s="160">
         <v>0.113</v>
       </c>
       <c r="O90" s="161">
-        <v>94.983314628615091</v>
+        <v>120.30091898433189</v>
       </c>
       <c r="P90" s="158">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="2:16">
@@ -11471,16 +11471,16 @@
         <v>417</v>
       </c>
       <c r="M91" s="159">
-        <v>0.43575000000000003</v>
+        <v>0.03</v>
       </c>
       <c r="N91" s="162">
         <v>0.113</v>
       </c>
       <c r="O91" s="163">
-        <v>120.30091898433189</v>
+        <v>94.983314628615091</v>
       </c>
       <c r="P91" s="159">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="2:16">
@@ -11616,7 +11616,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B24C1A-3B68-4220-852B-3FC4379CA807}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30803247-FBA9-480A-83D8-332DC8D2EC0B}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-27 02:26
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B154686-6FFE-4D4B-BC81-CEFB6225E4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{64040C98-5EDF-4590-AF47-CEC899E615DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -949,16 +949,16 @@
     <t>wind resource -- CF class won-ITA_25 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-ITA_25_c3</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_25 -- cost class 3</t>
+  </si>
+  <si>
     <t>e_won-ITA_25_c2</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_25 -- cost class 2</t>
-  </si>
-  <si>
-    <t>e_won-ITA_25_c3</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_25 -- cost class 3</t>
   </si>
   <si>
     <t>e_won-ITA_24_c2</t>
@@ -2497,7 +2497,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9C7D49D-5F2C-042F-93AC-B2AEEFA0F6F1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D83B01AA-23EE-6A8B-3ABB-46E694692E1F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2552,7 +2552,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA0FBF04-7A8D-516B-E7C4-F557F6857409}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBFC317D-6011-6538-476F-001ABF5127D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2607,7 +2607,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E147F068-388C-1801-3A46-F0787A9DD024}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35EE8D1A-D28E-5C53-4A23-47E1FCB8F05F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2662,7 +2662,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3A21777-3E92-7911-92B1-5D65FF82135A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{790C8EE5-2BD2-80CF-5750-E635515941D4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6592,7 +6592,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E7AFB4-6DC7-4E29-A846-2B9B38F1CB6F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18EF494-444E-4D8F-A08B-33C06AC41FD5}">
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7792,7 +7792,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{086C9CC9-DD47-408D-A42C-541955053A30}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{001456A7-802A-4C09-B559-D81A2D213E24}">
   <dimension ref="A1:P94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8683,16 +8683,16 @@
         <v>417</v>
       </c>
       <c r="M23" s="159">
-        <v>3.2032500000000002</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="N23" s="162">
         <v>0.245</v>
       </c>
       <c r="O23" s="163">
-        <v>42.969340484621256</v>
+        <v>107.03467623779731</v>
       </c>
       <c r="P23" s="159">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="2:16">
@@ -8724,16 +8724,16 @@
         <v>417</v>
       </c>
       <c r="M24" s="158">
-        <v>4.4999999999999997E-3</v>
+        <v>3.2032500000000002</v>
       </c>
       <c r="N24" s="160">
         <v>0.245</v>
       </c>
       <c r="O24" s="161">
-        <v>107.03467623779731</v>
+        <v>42.969340484621256</v>
       </c>
       <c r="P24" s="158">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="2:16">
@@ -11616,7 +11616,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B7C7F0-C638-48A6-8473-7D8FB11CA13F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAE6CC60-2AD4-41B0-B23B-6461F0773832}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-27 11:30
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64040C98-5EDF-4590-AF47-CEC899E615DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDEECC3E-FEA1-44ED-ABA2-593FB37B8697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2497,7 +2497,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D83B01AA-23EE-6A8B-3ABB-46E694692E1F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{791D730A-1AFF-B72F-932E-9C56196BD7A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2552,7 +2552,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBFC317D-6011-6538-476F-001ABF5127D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4BB63EA-6B09-19B0-326B-C2B9CCBDC233}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2607,7 +2607,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35EE8D1A-D28E-5C53-4A23-47E1FCB8F05F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDBEE083-546F-F37B-1E34-673057299BCF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2662,7 +2662,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{790C8EE5-2BD2-80CF-5750-E635515941D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D999A44C-53BD-1826-0EB6-B599E9CA541A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6592,7 +6592,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A18EF494-444E-4D8F-A08B-33C06AC41FD5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{598FCB13-47FA-4D27-8998-0EA50BC9919C}">
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7792,7 +7792,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{001456A7-802A-4C09-B559-D81A2D213E24}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF0CCA4-C630-4546-9800-1429B5DCB125}">
   <dimension ref="A1:P94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11616,7 +11616,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAE6CC60-2AD4-41B0-B23B-6461F0773832}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{887FE71D-0738-40F1-80EE-94667F3AF701}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-27 21:11
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDEECC3E-FEA1-44ED-ABA2-593FB37B8697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D2A43EF-874B-41B7-A221-D40BE1715CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1351,16 +1351,16 @@
     <t>wind resource -- CF class won-ITA_12 -- cost class 5</t>
   </si>
   <si>
+    <t>e_won-ITA_11_c4</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_11 -- cost class 4</t>
+  </si>
+  <si>
     <t>e_won-ITA_11_c2</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_11 -- cost class 2</t>
-  </si>
-  <si>
-    <t>e_won-ITA_11_c4</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_11 -- cost class 4</t>
   </si>
   <si>
     <t>e_won-ITA_11_c1</t>
@@ -2497,7 +2497,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{791D730A-1AFF-B72F-932E-9C56196BD7A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8914948-6DA8-DBE1-6C18-E5F916692B36}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2552,7 +2552,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4BB63EA-6B09-19B0-326B-C2B9CCBDC233}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88B02A1C-0A26-6DEB-9D06-6D2845BCA531}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2607,7 +2607,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDBEE083-546F-F37B-1E34-673057299BCF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3BE713B-6747-D56E-EE41-65E535542A9A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2662,7 +2662,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D999A44C-53BD-1826-0EB6-B599E9CA541A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{335F76D5-70BD-991E-E1FC-26AA87CC5238}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6592,7 +6592,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{598FCB13-47FA-4D27-8998-0EA50BC9919C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8C697C6-B4A2-4A0D-A719-6AF91BC6F17F}">
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7792,7 +7792,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF0CCA4-C630-4546-9800-1429B5DCB125}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58B8F73-51DC-4C17-B220-AFAD6FB666F9}">
   <dimension ref="A1:P94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11430,16 +11430,16 @@
         <v>417</v>
       </c>
       <c r="M90" s="158">
-        <v>0.03</v>
+        <v>0.43575000000000003</v>
       </c>
       <c r="N90" s="160">
         <v>0.113</v>
       </c>
       <c r="O90" s="161">
-        <v>94.983314628615091</v>
+        <v>120.30091898433189</v>
       </c>
       <c r="P90" s="158">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="2:16">
@@ -11471,16 +11471,16 @@
         <v>417</v>
       </c>
       <c r="M91" s="159">
-        <v>0.43575000000000003</v>
+        <v>0.03</v>
       </c>
       <c r="N91" s="162">
         <v>0.113</v>
       </c>
       <c r="O91" s="163">
-        <v>120.30091898433189</v>
+        <v>94.983314628615091</v>
       </c>
       <c r="P91" s="159">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="2:16">
@@ -11616,7 +11616,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{887FE71D-0738-40F1-80EE-94667F3AF701}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBEABAD5-4E44-4A45-9F71-87703170EE12}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-08-30 01:00
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECE5DFC5-65BC-45DC-AF4C-64EA90304840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DEF1CD09-A796-47DC-80C1-1BC0A5716BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -853,18 +853,18 @@
     <t>wind resource -- CF class won-ITA_33 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-ITA_32_c3</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_32 -- cost class 3</t>
+  </si>
+  <si>
     <t>e_won-ITA_32_c1</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_32 -- cost class 1</t>
   </si>
   <si>
-    <t>e_won-ITA_32_c3</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_32 -- cost class 3</t>
-  </si>
-  <si>
     <t>e_won-ITA_32_c2</t>
   </si>
   <si>
@@ -949,16 +949,16 @@
     <t>wind resource -- CF class won-ITA_25 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-ITA_25_c3</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-ITA_25 -- cost class 3</t>
+  </si>
+  <si>
     <t>e_won-ITA_25_c2</t>
   </si>
   <si>
     <t>wind resource -- CF class won-ITA_25 -- cost class 2</t>
-  </si>
-  <si>
-    <t>e_won-ITA_25_c3</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-ITA_25 -- cost class 3</t>
   </si>
   <si>
     <t>e_won-ITA_24_c2</t>
@@ -2497,7 +2497,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDE97D37-D8B8-2D73-B21A-CE57ECB0E5A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{343B99DC-92EC-5942-D7B6-3C8834D0F22B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2552,7 +2552,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4B5BC4A-0A05-D494-A2CA-BE82E5AE6BD2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F079502C-41D6-AECC-F54C-4133F22B0092}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2607,7 +2607,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59FD31C5-FAE9-3AA5-67CA-BE11F1FBC934}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C36D4AC-D9C7-1E32-8FC5-454C25144A9A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2662,7 +2662,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{689A4E60-DC83-0DD5-7A0A-35FC9E90C0D8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBD90FBE-5965-7B01-D736-4BFE51E56865}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6592,7 +6592,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6115380-A2E0-40D6-94E2-F5EF4D006D63}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC352F26-178F-4075-8BA1-2F87C8DA8BD4}">
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7792,7 +7792,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{330BA2FF-B0B0-4F22-9C62-A9BD1A83EE07}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60AFA001-AC6F-481A-B3D2-E1DC644315DB}">
   <dimension ref="A1:P94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8027,16 +8027,16 @@
         <v>417</v>
       </c>
       <c r="M7" s="159">
-        <v>1.5E-3</v>
+        <v>2.4990000000000001</v>
       </c>
       <c r="N7" s="162">
         <v>0.32200000000000001</v>
       </c>
       <c r="O7" s="163">
-        <v>31.372355844942916</v>
+        <v>39.630069093581724</v>
       </c>
       <c r="P7" s="159">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -8068,16 +8068,16 @@
         <v>417</v>
       </c>
       <c r="M8" s="158">
-        <v>2.4990000000000001</v>
+        <v>1.5E-3</v>
       </c>
       <c r="N8" s="160">
         <v>0.32200000000000001</v>
       </c>
       <c r="O8" s="161">
-        <v>39.630069093581724</v>
+        <v>31.372355844942916</v>
       </c>
       <c r="P8" s="158">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -8683,16 +8683,16 @@
         <v>417</v>
       </c>
       <c r="M23" s="159">
-        <v>3.2032500000000002</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="N23" s="162">
         <v>0.245</v>
       </c>
       <c r="O23" s="163">
-        <v>42.969340484621256</v>
+        <v>107.03467623779731</v>
       </c>
       <c r="P23" s="159">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="2:16">
@@ -8724,16 +8724,16 @@
         <v>417</v>
       </c>
       <c r="M24" s="158">
-        <v>4.4999999999999997E-3</v>
+        <v>3.2032500000000002</v>
       </c>
       <c r="N24" s="160">
         <v>0.245</v>
       </c>
       <c r="O24" s="161">
-        <v>107.03467623779731</v>
+        <v>42.969340484621256</v>
       </c>
       <c r="P24" s="158">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="2:16">
@@ -11616,7 +11616,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB19AA4-CF2A-4DC0-812B-01C6605AFDE1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D85FE3-ED5B-4E67-8A11-F04F46332348}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 01:34
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F0ED6EC-F821-4A6B-BAB4-7774DEB5914E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{76DF49F8-83EF-44ED-8951-6697D24C2F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3952,7 +3952,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6150EF95-77F2-7DDD-FFBE-CC45544176B7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FAE4E9B-A37A-47A1-C476-E797AD1C62DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4007,7 +4007,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23E32F63-C856-C92E-88AE-CC3DF6C319C7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{602D22E6-4BE3-1531-2912-459836BCFEF6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4062,7 +4062,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{689DDD02-5DE4-ED56-247E-5DFAA27453CF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C595D5A-86AA-3CDD-2EC3-FF3262591753}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4117,7 +4117,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EE312F3-6976-62EE-31B4-664E50B07B12}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D155B3D7-A144-C012-5DA2-A69BF00F75F4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8047,7 +8047,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB656918-0691-4454-A826-FD3F75D20659}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAEA6CEC-E1B7-4466-8E75-AE2FE8D4B3A1}">
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9655,7 +9655,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174C6C44-C8B6-4A0E-B85A-98AF2779E6EB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5205E0B-184A-482F-8E30-092E8C4E3BDB}">
   <dimension ref="A1:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21638,7 +21638,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{686A12DB-4AB6-4D3D-8C34-106C8F94FC2A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADC47A-2535-4E66-8B7B-1BCB754E5D95}">
   <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 09:30
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A6D3FCB-01BB-4D80-85F1-86382E1495DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DFD4E9A-CA48-42B5-B2E5-2EC93F2755F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7729,7 +7729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667280C2-4562-40F1-901D-1670CB46EB0F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{580E1426-AE54-4CD1-AB3E-69F1DB116AC2}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9308,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A2773D-9538-409C-B6CD-E80C57E35AC5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48CDC65C-CE69-469F-9060-38D18A48D88F}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21253,7 +21253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E966BE4-4674-46E0-9403-C04B9F949B88}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9AFDD2-2822-4D8E-BD9B-51A145A42D1F}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 12:40
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DFD4E9A-CA48-42B5-B2E5-2EC93F2755F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB910579-E4B0-4F16-A42B-32FA95AB15BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7729,7 +7729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{580E1426-AE54-4CD1-AB3E-69F1DB116AC2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14CCBB58-834E-4625-8262-80F4A8086253}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9308,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48CDC65C-CE69-469F-9060-38D18A48D88F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A31881-D7DA-4CD5-855A-6BA01A12CB2A}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21253,7 +21253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9AFDD2-2822-4D8E-BD9B-51A145A42D1F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C1DA18-05B8-4C3B-A809-10F75B17A82F}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 12:44
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB910579-E4B0-4F16-A42B-32FA95AB15BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E94C2B2E-B5BE-4AC5-B279-7EA46C66F38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7729,7 +7729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14CCBB58-834E-4625-8262-80F4A8086253}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA089E8-0974-4FD3-82E2-C9F9E8AF33C3}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9308,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A31881-D7DA-4CD5-855A-6BA01A12CB2A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB034FE-C973-418A-A628-96C81107A442}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21253,7 +21253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C1DA18-05B8-4C3B-A809-10F75B17A82F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{713A52EA-E54B-4B5F-917E-81FFA5A85F52}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 13:01
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E94C2B2E-B5BE-4AC5-B279-7EA46C66F38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{87BF04F5-5EF2-407F-9993-BBE19711481A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7729,7 +7729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA089E8-0974-4FD3-82E2-C9F9E8AF33C3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F46CAF89-CCCF-4ED6-88F4-0D2534CED8F7}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9308,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB034FE-C973-418A-A628-96C81107A442}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BBA17F8-A8E7-4817-BF12-7778AB1A92F3}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21253,7 +21253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{713A52EA-E54B-4B5F-917E-81FFA5A85F52}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D0DFA0-8917-4B6C-A211-F8E1DFDC96B8}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 13:43
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87BF04F5-5EF2-407F-9993-BBE19711481A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8724FC4-C658-4344-B87D-7CDC7CF7205E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7729,7 +7729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F46CAF89-CCCF-4ED6-88F4-0D2534CED8F7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31304136-2D6A-4946-9919-63FD28B1FA64}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9308,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BBA17F8-A8E7-4817-BF12-7778AB1A92F3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6236C74F-0A7A-4935-8891-E8E213DA4EE0}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21253,7 +21253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D0DFA0-8917-4B6C-A211-F8E1DFDC96B8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA78A12-931D-4CC5-A104-770670C8DBEE}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 13:46
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8724FC4-C658-4344-B87D-7CDC7CF7205E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{43E55711-04A4-4E2D-9AB9-B49F157396C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7729,7 +7729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31304136-2D6A-4946-9919-63FD28B1FA64}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{841137D9-1D1D-4BA6-ADC5-D92D481231B9}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9308,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6236C74F-0A7A-4935-8891-E8E213DA4EE0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4856C1F5-6CB1-443E-88B4-CB0B28096582}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21253,7 +21253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA78A12-931D-4CC5-A104-770670C8DBEE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC59E72A-7C3D-4371-B9FB-739748C2CA0B}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 16:38
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35796A25-453D-4A2A-80AC-C8C62EE8DC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{58E2B3BD-2BC7-4A1D-A368-A670CAE50920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7729,7 +7729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C01EC95-A9E2-4004-8325-E1FA92F26F27}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2D470F-9226-4B4C-A1FE-C89ADA6276B9}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9308,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAC344A3-ED6C-43EC-9F91-A1D6B878F192}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB9B944-B843-47FB-B10F-0EFAC1FA98EF}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21253,7 +21253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C118148-2165-4E90-A0BB-BF7D0D445FA5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B6D465-6C4D-4FF0-B0BD-84840EBB9F2A}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 16:47
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58E2B3BD-2BC7-4A1D-A368-A670CAE50920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE333B9E-05F0-480C-96BC-17573FCADA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7729,7 +7729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2D470F-9226-4B4C-A1FE-C89ADA6276B9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E982BD4-36E7-42B4-99B7-24479EB5EE9A}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9308,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB9B944-B843-47FB-B10F-0EFAC1FA98EF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C65985C-437D-47FA-8958-728A606131B9}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21253,7 +21253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B6D465-6C4D-4FF0-B0BD-84840EBB9F2A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC6C0F27-06B3-45F0-8FC1-B3A0AFE8D3B2}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 17:13
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE333B9E-05F0-480C-96BC-17573FCADA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{90C4DEBF-129D-4F22-BD33-193DC1704B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7729,7 +7729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E982BD4-36E7-42B4-99B7-24479EB5EE9A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D53F28E0-335F-4B25-9BFD-6A933144C4D7}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9308,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C65985C-437D-47FA-8958-728A606131B9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5554B4BB-06C0-4275-B4A4-BF8967DC69C1}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21253,7 +21253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC6C0F27-06B3-45F0-8FC1-B3A0AFE8D3B2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06DDB56-C20E-481D-A2F3-971B4A66BB0E}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 18:33
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{90C4DEBF-129D-4F22-BD33-193DC1704B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FC8817C-5B4C-466A-A632-55B1C251C0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7729,7 +7729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D53F28E0-335F-4B25-9BFD-6A933144C4D7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1350BBD5-6B88-4B0E-AAF0-3C5B9E3B195B}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9308,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5554B4BB-06C0-4275-B4A4-BF8967DC69C1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0687CB1-1E6D-4E63-96AA-0B430D243EA9}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21253,7 +21253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06DDB56-C20E-481D-A2F3-971B4A66BB0E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F633EAD9-E050-46F5-BACF-57AC3891F70F}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 18:45
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FC8817C-5B4C-466A-A632-55B1C251C0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{15AB0699-9A8E-4C46-9B01-54A1065E9936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7729,7 +7729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1350BBD5-6B88-4B0E-AAF0-3C5B9E3B195B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107FACF6-8FC2-44DB-95CE-1F2CD36B234E}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9308,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0687CB1-1E6D-4E63-96AA-0B430D243EA9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C429FB-DB37-4F55-9DB7-F8264C5DFDBE}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21253,7 +21253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F633EAD9-E050-46F5-BACF-57AC3891F70F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4765403F-416A-4FB5-9EF7-4C9440A3C8D6}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 19:16
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15AB0699-9A8E-4C46-9B01-54A1065E9936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1906982C-D2D5-4477-9058-54B164E36E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7729,7 +7729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107FACF6-8FC2-44DB-95CE-1F2CD36B234E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A8CDC2-E512-4E3D-9029-3C222BB391B1}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9308,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C429FB-DB37-4F55-9DB7-F8264C5DFDBE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1240F954-0A0F-4CA1-89D0-E24EA54C18F7}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21253,7 +21253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4765403F-416A-4FB5-9EF7-4C9440A3C8D6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04AA423-DAB6-457D-AC0F-D3FFD8CCFF2C}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 19:20
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1906982C-D2D5-4477-9058-54B164E36E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2AEAC2B-9780-464B-8FB7-6060165128CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7729,7 +7729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A8CDC2-E512-4E3D-9029-3C222BB391B1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D71CD372-089D-44DF-B0FF-2EFC2CE77222}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9308,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1240F954-0A0F-4CA1-89D0-E24EA54C18F7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36FDC788-B6AD-4420-8CAE-D9C851A8276D}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21253,7 +21253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04AA423-DAB6-457D-AC0F-D3FFD8CCFF2C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE934A7-A758-46F0-BC96-A7BCA31812D5}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 19:42
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2AEAC2B-9780-464B-8FB7-6060165128CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0B2E224-3616-4907-BFD5-F70C91665CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7729,7 +7729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D71CD372-089D-44DF-B0FF-2EFC2CE77222}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5918423-4C18-4641-80FE-921CD20D3D48}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9308,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36FDC788-B6AD-4420-8CAE-D9C851A8276D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79DDA68-F156-4914-B2BA-28B753FB33AC}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21253,7 +21253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE934A7-A758-46F0-BC96-A7BCA31812D5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C9F2F7-5CF2-4173-9861-62C091761134}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 19:53
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0B2E224-3616-4907-BFD5-F70C91665CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{27AC6CDF-4040-45BB-BA28-972EAF48DEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7729,7 +7729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5918423-4C18-4641-80FE-921CD20D3D48}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C320662-A8D8-40B7-9431-D381078FB62C}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9308,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79DDA68-F156-4914-B2BA-28B753FB33AC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2605C97C-12CB-4B2F-B437-D3B5B4E81D9F}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21253,7 +21253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C9F2F7-5CF2-4173-9861-62C091761134}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B897419-AFFA-4987-9611-3C969F7D2BB5}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 20:03
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27AC6CDF-4040-45BB-BA28-972EAF48DEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC1144DE-E5DC-4C88-A86B-DA43183F1F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7729,7 +7729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C320662-A8D8-40B7-9431-D381078FB62C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F39672-ECAD-44ED-BDE2-5C8F35AA48D9}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9308,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2605C97C-12CB-4B2F-B437-D3B5B4E81D9F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC18CD5F-F624-48EE-A2EA-DDB4B3DC93F5}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21253,7 +21253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B897419-AFFA-4987-9611-3C969F7D2BB5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A790278-B9BC-4235-9DC8-693A3A4F544A}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 20:46
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC1144DE-E5DC-4C88-A86B-DA43183F1F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{91A98A4F-B84D-447D-B79C-76D0E17B9F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7729,7 +7729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F39672-ECAD-44ED-BDE2-5C8F35AA48D9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B20549D-DD23-49D6-AAB8-7CC5416F93CB}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9308,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC18CD5F-F624-48EE-A2EA-DDB4B3DC93F5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4B724A-8F5D-47EE-BC75-DD476A44AA75}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21253,7 +21253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A790278-B9BC-4235-9DC8-693A3A4F544A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FBB252-7370-48BB-84A6-45653163A06E}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 20:53
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91A98A4F-B84D-447D-B79C-76D0E17B9F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F24286B-8892-426E-8DBD-C74B5034F5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7729,7 +7729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B20549D-DD23-49D6-AAB8-7CC5416F93CB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4ED87D-9907-4D08-A919-62BD72FF63D8}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9308,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4B724A-8F5D-47EE-BC75-DD476A44AA75}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0302B809-1746-409B-A1F0-1939FF2AF72C}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21253,7 +21253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5FBB252-7370-48BB-84A6-45653163A06E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18DCE692-C7B8-4D1F-9205-AC31A37B9437}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-01 21:50
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F24286B-8892-426E-8DBD-C74B5034F5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D127597D-AEE5-48F8-992B-CCFC3E29B31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7729,7 +7729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4ED87D-9907-4D08-A919-62BD72FF63D8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A25FDF9-D0D6-40E5-B953-B5A0C2AEE983}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9308,7 +9308,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0302B809-1746-409B-A1F0-1939FF2AF72C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB1D0E1-C1A3-40A4-98D2-61FE1CCA4F57}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21253,7 +21253,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18DCE692-C7B8-4D1F-9205-AC31A37B9437}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B2BEAF-D4D3-4A04-9458-607599A2DECA}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-04 12:45
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{316A63CD-5BB8-45AB-A1EB-DF51D3B57A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{00696181-156F-4E35-8C76-B98DF356D1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7821,7 +7821,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03B6C33-E5DF-4B19-B5F4-65915581BD2F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FBDA63-F171-4334-BB2D-48813A9A9438}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9400,7 +9400,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BC4CB4-B9E2-4F8F-9630-E0A57BBF9485}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76495FB6-9600-49BC-833E-B326C84D235E}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21345,7 +21345,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A957D316-92E3-4831-B54D-8E1A905DB344}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A05930C8-7DED-43A1-A340-678D8C73A2BC}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-05 17:03
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25542E7D-EC9D-4017-B105-7F3B8F3F40BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A345BD1-B128-46A9-891E-250E73B37D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7821,7 +7821,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04725BE-7B5C-4F46-AF69-4AE1A2B906DB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E65313FA-AADA-40BA-A0B1-E65E9ACD9580}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9400,7 +9400,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E42C30D2-3138-40FD-A17A-F60E4D234546}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619D80F3-48EB-4A8E-83D1-48E90D62ECDF}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21345,7 +21345,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C7B9505-FD1D-4AD2-A81D-A45CC7791222}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A20DC1D-DA63-47A9-B9E5-8F1879993D0C}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-05 19:26
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A345BD1-B128-46A9-891E-250E73B37D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBF4121D-35A9-4BE3-8BE5-F054108E62BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7821,7 +7821,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E65313FA-AADA-40BA-A0B1-E65E9ACD9580}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD2F010-27A7-4504-8FF9-FC88A6707454}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9400,7 +9400,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619D80F3-48EB-4A8E-83D1-48E90D62ECDF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3AC430-CD52-487D-BABB-1C0C798AF8AF}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21345,7 +21345,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A20DC1D-DA63-47A9-B9E5-8F1879993D0C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FDDD8C-200B-4F5B-BA34-9652C48578BB}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-05 21:00
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBF4121D-35A9-4BE3-8BE5-F054108E62BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{83B56C0E-95A7-41C1-97C3-1BF2975F87E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7821,7 +7821,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD2F010-27A7-4504-8FF9-FC88A6707454}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40CC50F9-7DF4-438A-8AF6-027E9DA1ADB6}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9400,7 +9400,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3AC430-CD52-487D-BABB-1C0C798AF8AF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E57037DC-B9EF-4DA3-A1DE-C06F66BA84CA}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21345,7 +21345,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FDDD8C-200B-4F5B-BA34-9652C48578BB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A3C7180-75C0-4977-A4EF-CAA335AC9F33}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ITA model - 2025-09-05 21:23
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_ITA/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83B56C0E-95A7-41C1-97C3-1BF2975F87E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC493FE8-ADA1-498B-9641-F98BE24C6BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7821,7 +7821,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40CC50F9-7DF4-438A-8AF6-027E9DA1ADB6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6068149F-B299-4753-A993-20299A779693}">
   <dimension ref="B9:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9400,7 +9400,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E57037DC-B9EF-4DA3-A1DE-C06F66BA84CA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FB7BFD1-36F0-4F2D-B70E-827707DA4A7F}">
   <dimension ref="B9:AB172"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21345,7 +21345,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A3C7180-75C0-4977-A4EF-CAA335AC9F33}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC16FD52-78AA-41E5-BC55-4D1076743466}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>